<commit_message>
allow tony and quilladin
</commit_message>
<xml_diff>
--- a/batch_demo.xlsx
+++ b/batch_demo.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26819"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3080" yWindow="640" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -22,69 +18,69 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Compute</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Image</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Degradation</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ParDeg1</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ParDeg2</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Restoration</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ParRes1</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ParRes2</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Descriptor</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Output</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>quilladin</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blind</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>nothing</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>LBP</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>auto</t>
-    <phoneticPr fontId="0" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -116,10 +112,10 @@
     </xf>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -410,14 +406,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -456,16 +450,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -483,14 +477,457 @@
         <v>13</v>
       </c>
     </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>13</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>19</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>23</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>25</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>27</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>29</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>31</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="0" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor change to batch
</commit_message>
<xml_diff>
--- a/batch_demo.xlsx
+++ b/batch_demo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Compute</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -143,8 +143,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -169,13 +187,19 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="13">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -468,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -590,6 +614,44 @@
         <v>12</v>
       </c>
       <c r="L3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
works with * in io_series
</commit_message>
<xml_diff>
--- a/batch_demo.xlsx
+++ b/batch_demo.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>Compute</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -84,12 +84,6 @@
   </si>
   <si>
     <t>blurred</t>
-  </si>
-  <si>
-    <t>med</t>
-  </si>
-  <si>
-    <t>comparison</t>
   </si>
 </sst>
 </file>
@@ -143,8 +137,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -187,19 +193,23 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="17">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -492,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -587,16 +597,16 @@
         <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
         <v>3</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -622,7 +632,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -631,7 +641,7 @@
         <v>14</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -652,6 +662,120 @@
         <v>12</v>
       </c>
       <c r="L4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
print to outer csv
</commit_message>
<xml_diff>
--- a/batch_demo.xlsx
+++ b/batch_demo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24820" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="-760" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <dimension ref="A1:L1233"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>